<commit_message>
Code tweaks, adding of activities and remove dead code
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/no_activity_sheet.xlsx
+++ b/tests/integration_test_files/no_activity_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20189C81-9062-114E-A014-9BF7BD253861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07E4B58-0949-8947-83EE-B67A2F381473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35040" yWindow="3820" windowWidth="33260" windowHeight="19480" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="35040" yWindow="3820" windowWidth="33260" windowHeight="19480" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -19,15 +19,16 @@
     <sheet name="studyDesignArms" sheetId="15" r:id="rId4"/>
     <sheet name="studyDesignEpochs" sheetId="14" r:id="rId5"/>
     <sheet name="mainTimeline" sheetId="1" r:id="rId6"/>
-    <sheet name="studyDesignInterventions" sheetId="16" r:id="rId7"/>
-    <sheet name="studyDesignIndications" sheetId="6" r:id="rId8"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId9"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId10"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId11"/>
-    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId12"/>
-    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId13"/>
-    <sheet name="studyDesignElements" sheetId="13" r:id="rId14"/>
-    <sheet name="configuration" sheetId="10" r:id="rId15"/>
+    <sheet name="studyDesignTiming" sheetId="17" r:id="rId7"/>
+    <sheet name="studyDesignInterventions" sheetId="16" r:id="rId8"/>
+    <sheet name="studyDesignIndications" sheetId="6" r:id="rId9"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId10"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId11"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId12"/>
+    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId13"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId14"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId15"/>
+    <sheet name="configuration" sheetId="10" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,10 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="322">
-  <si>
-    <t>Epoch</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="348">
   <si>
     <t>Screening</t>
   </si>
@@ -61,15 +59,6 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>Cycle</t>
-  </si>
-  <si>
-    <t>Cycle End Rule</t>
-  </si>
-  <si>
-    <t>A:</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -79,9 +68,6 @@
     <t>Child Activity</t>
   </si>
   <si>
-    <t>N: 0..2 Days</t>
-  </si>
-  <si>
     <t>Demographics</t>
   </si>
   <si>
@@ -94,36 +80,12 @@
     <t>15 min</t>
   </si>
   <si>
-    <t>P: +24 Hours</t>
-  </si>
-  <si>
-    <t>0..4 Hours</t>
-  </si>
-  <si>
-    <t>N: Pre Dose</t>
-  </si>
-  <si>
     <t>Day 24</t>
   </si>
   <si>
     <t>Day 35</t>
   </si>
   <si>
-    <t>P: +7 Days</t>
-  </si>
-  <si>
-    <t>-3..3 Days</t>
-  </si>
-  <si>
-    <t>First Cycle Start</t>
-  </si>
-  <si>
-    <t>Cycle Period</t>
-  </si>
-  <si>
-    <t>Timing</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -649,12 +611,6 @@
     <t>E5</t>
   </si>
   <si>
-    <t>Encounter xref</t>
-  </si>
-  <si>
-    <t>Window</t>
-  </si>
-  <si>
     <t>BC/Procedure/Timeline</t>
   </si>
   <si>
@@ -1016,6 +972,129 @@
   </si>
   <si>
     <t>31 .. 70 years</t>
+  </si>
+  <si>
+    <t>SCREEN</t>
+  </si>
+  <si>
+    <t>PRE DOSE</t>
+  </si>
+  <si>
+    <t>DOSE</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>FU</t>
+  </si>
+  <si>
+    <t>Pre Dose</t>
+  </si>
+  <si>
+    <t>Dosing</t>
+  </si>
+  <si>
+    <t>Day 14</t>
+  </si>
+  <si>
+    <t>Screen</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>(EXIT)</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>epoch</t>
+  </si>
+  <si>
+    <t>encounter</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>timingValue</t>
+  </si>
+  <si>
+    <t>toFrom</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>TIM1</t>
+  </si>
+  <si>
+    <t>Screening timing</t>
+  </si>
+  <si>
+    <t>BEFORE</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>S2S</t>
+  </si>
+  <si>
+    <t>TIM2</t>
+  </si>
+  <si>
+    <t>Pre dose timing</t>
+  </si>
+  <si>
+    <t>Pre dose</t>
+  </si>
+  <si>
+    <t>0..4 hours</t>
+  </si>
+  <si>
+    <t>TIM3</t>
+  </si>
+  <si>
+    <t>Dosing anchor</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>1 Day</t>
+  </si>
+  <si>
+    <t>TIM4</t>
+  </si>
+  <si>
+    <t>24 Hour timing</t>
+  </si>
+  <si>
+    <t>AFTER</t>
+  </si>
+  <si>
+    <t>24 Hours</t>
+  </si>
+  <si>
+    <t>TIM5</t>
+  </si>
+  <si>
+    <t>Follow up timing</t>
+  </si>
+  <si>
+    <t>7 Days</t>
+  </si>
+  <si>
+    <t>-3..3 days</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1157,13 +1236,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1183,9 +1259,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1223,7 +1299,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1329,7 +1405,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1471,7 +1547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1498,10 +1574,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -1510,10 +1586,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
@@ -1522,10 +1598,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
@@ -1534,10 +1610,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
@@ -1546,10 +1622,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
@@ -1558,10 +1634,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
@@ -1570,10 +1646,10 @@
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
@@ -1582,10 +1658,10 @@
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="E8"/>
       <c r="F8"/>
@@ -1594,52 +1670,52 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
       <c r="H9" s="19" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -1648,10 +1724,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -1660,10 +1736,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -1706,6 +1782,95 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="8.5" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.5" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>120</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" t="s">
+        <v>303</v>
+      </c>
+      <c r="G4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:K36"/>
   <sheetViews>
@@ -1729,85 +1894,85 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -1816,16 +1981,16 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1834,16 +1999,16 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1852,16 +2017,16 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1870,16 +2035,16 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1888,16 +2053,16 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -1906,16 +2071,16 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1924,16 +2089,16 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -1942,16 +2107,16 @@
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -1960,16 +2125,16 @@
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1978,16 +2143,16 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -2272,7 +2437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -2292,90 +2457,90 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="E5" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2383,7 +2548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D608A778-255D-4443-A7EA-03049F1FC98F}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -2404,65 +2569,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D3" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E3" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="G3" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2475,7 +2640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -2495,137 +2660,137 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2634,7 +2799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D84F3-D0D8-A149-BA12-7DBD407EC782}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -2652,104 +2817,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>223</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2758,7 +2923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2773,18 +2938,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2811,62 +2976,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -2891,10 +3056,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -2902,10 +3067,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -2913,43 +3078,43 @@
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+        <v>32</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+        <v>33</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+        <v>34</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -2957,10 +3122,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -2968,10 +3133,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
@@ -2979,10 +3144,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
@@ -2990,7 +3155,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -2999,53 +3164,53 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3062,16 +3227,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3096,53 +3261,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3170,57 +3335,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3236,13 +3401,13 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10:B11"/>
+      <selection pane="bottomRight" sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
     <col min="4" max="8" width="12.33203125" style="1" customWidth="1"/>
     <col min="9" max="10" width="10.83203125" style="1"/>
@@ -3250,258 +3415,435 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>243</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>312</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>313</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>314</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>21</v>
+        <v>252</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>315</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>314</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>24</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="15"/>
       <c r="C4" s="15" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="15"/>
       <c r="C5" s="15" t="s">
-        <v>4</v>
+        <v>317</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>308</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>309</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>310</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>311</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="15"/>
       <c r="C6" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="15" t="s">
-        <v>199</v>
+        <v>320</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>195</v>
+        <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>196</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>197</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>198</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2"/>
+        <v>321</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>184</v>
+      </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F1:G1"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC2826C-C481-A544-B189-16EC281699E9}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="9" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="E2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G2" t="s">
+        <v>330</v>
+      </c>
+      <c r="H2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>331</v>
+      </c>
+      <c r="I3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" t="s">
+        <v>338</v>
+      </c>
+      <c r="E4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F4" t="s">
+        <v>309</v>
+      </c>
+      <c r="G4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B5" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E5" t="s">
+        <v>310</v>
+      </c>
+      <c r="F5" t="s">
+        <v>309</v>
+      </c>
+      <c r="G5" t="s">
+        <v>343</v>
+      </c>
+      <c r="H5" t="s">
+        <v>331</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" t="s">
+        <v>342</v>
+      </c>
+      <c r="E6" t="s">
+        <v>311</v>
+      </c>
+      <c r="F6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G6" t="s">
+        <v>346</v>
+      </c>
+      <c r="H6" t="s">
+        <v>331</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3617E1F-BE32-EB42-AF4A-86B4395F9829}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -3535,179 +3877,179 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="22" t="s">
         <v>258</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="22" t="s">
+      <c r="H1" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="P1" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>272</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>276</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>278</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>279</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>281</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>282</v>
-      </c>
       <c r="Q1" s="22" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="S1" s="22" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="G2" t="s">
+        <v>276</v>
+      </c>
+      <c r="H2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I2" t="s">
+        <v>278</v>
+      </c>
+      <c r="J2" t="s">
+        <v>279</v>
+      </c>
+      <c r="K2" t="s">
+        <v>280</v>
+      </c>
+      <c r="L2" t="s">
+        <v>281</v>
+      </c>
+      <c r="M2" t="s">
+        <v>282</v>
+      </c>
+      <c r="N2" t="s">
+        <v>283</v>
+      </c>
+      <c r="O2" t="s">
+        <v>284</v>
+      </c>
+      <c r="P2" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>159</v>
+      </c>
+      <c r="R2" t="s">
         <v>286</v>
       </c>
-      <c r="C2" t="s">
+      <c r="S2" s="24" t="s">
         <v>287</v>
-      </c>
-      <c r="D2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E2" t="s">
-        <v>289</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>290</v>
-      </c>
-      <c r="G2" t="s">
-        <v>291</v>
-      </c>
-      <c r="H2" t="s">
-        <v>292</v>
-      </c>
-      <c r="I2" t="s">
-        <v>293</v>
-      </c>
-      <c r="J2" t="s">
-        <v>294</v>
-      </c>
-      <c r="K2" t="s">
-        <v>295</v>
-      </c>
-      <c r="L2" t="s">
-        <v>296</v>
-      </c>
-      <c r="M2" t="s">
-        <v>297</v>
-      </c>
-      <c r="N2" t="s">
-        <v>298</v>
-      </c>
-      <c r="O2" t="s">
-        <v>299</v>
-      </c>
-      <c r="P2" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>172</v>
-      </c>
-      <c r="R2" t="s">
-        <v>301</v>
-      </c>
-      <c r="S2" s="24" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="C3" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="D3" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="E3" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="G3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H3" t="s">
         <v>291</v>
       </c>
-      <c r="H3" t="s">
-        <v>306</v>
-      </c>
       <c r="I3" t="s">
+        <v>278</v>
+      </c>
+      <c r="J3" t="s">
+        <v>292</v>
+      </c>
+      <c r="K3" t="s">
         <v>293</v>
       </c>
-      <c r="J3" t="s">
-        <v>307</v>
-      </c>
-      <c r="K3" t="s">
-        <v>308</v>
-      </c>
       <c r="L3" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="M3" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="N3" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="O3" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="P3" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="Q3" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="R3" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="S3" s="24" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -3715,7 +4057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3732,133 +4074,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="C3" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="8.5" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="24.5" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>312</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>313</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>319</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>120</v>
-      </c>
-      <c r="H2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>316</v>
-      </c>
-      <c r="B3" t="s">
-        <v>317</v>
-      </c>
-      <c r="G3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>316</v>
-      </c>
-      <c r="B4" t="s">
-        <v>318</v>
-      </c>
-      <c r="G4" t="s">
-        <v>321</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>